<commit_message>
Added a couple of Brown names to the nucleus dictionary
</commit_message>
<xml_diff>
--- a/nucleusDictionary.xlsx
+++ b/nucleusDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\claptrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B8CDEC-07A6-4B79-B3F1-F920DE915026}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF0FF88-A024-49F3-A463-76D9DF0A6F6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D8785CB6-C8D8-40FF-ADCB-2295CEE1095E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4364" uniqueCount="1728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4376" uniqueCount="1730">
   <si>
     <t>Noun</t>
   </si>
@@ -5215,6 +5215,12 @@
   </si>
   <si>
     <t>Person</t>
+  </si>
+  <si>
+    <t>Chris Brown</t>
+  </si>
+  <si>
+    <t>James Brown</t>
   </si>
 </sst>
 </file>
@@ -5319,8 +5325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E165EFC-BDFB-4E89-BB21-4AEB42E5959B}" name="Table1" displayName="Table1" ref="A1:BG799" totalsRowShown="0">
-  <autoFilter ref="A1:BG799" xr:uid="{0151B548-B959-4AF4-A55C-85BB33381FBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E165EFC-BDFB-4E89-BB21-4AEB42E5959B}" name="Table1" displayName="Table1" ref="A1:BG801" totalsRowShown="0">
+  <autoFilter ref="A1:BG801" xr:uid="{0151B548-B959-4AF4-A55C-85BB33381FBD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BG639">
     <sortCondition ref="Q1:Q639"/>
   </sortState>
@@ -5714,10 +5720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F47E38D-BE92-4C7C-9041-C9D3F2525834}">
-  <dimension ref="A1:BG799"/>
+  <dimension ref="A1:BG801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="AG341" sqref="AG341"/>
+    <sheetView tabSelected="1" topLeftCell="A766" workbookViewId="0">
+      <selection activeCell="AH794" sqref="AH794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65412,6 +65418,160 @@
         <v>1726</v>
       </c>
     </row>
+    <row r="800" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A800" t="str">
+        <f>CONCATENATE("{""spelling"": """,Q800,""", ""group"": """,O800,""", ""pos"": """,S800,""", ""form"": """,T800,""", ""adult"": ",IF(R800=TRUE,"true","false"),", ""has"": [",B800,"]",", ""in"": [",C800,"]",", ""on"": [",D800,"]",", ""from"": [",E800,"]",", ""is"": [",F800,"]",", ""typeOf"": [",G800,"]",", ""supertypeOf"": [",H800,"]",", ""nearlyIs"": [",I800,"]",", ""property"": [",J800,"]",", ""acts"": [",K800,"]",", ""actsCont"": [",L800,"]",", ""recipient"": [",M800,"]",", ""recipientPast"": [",N800,"]},")</f>
+        <v>{"spelling": "Chris Brown", "group": "", "pos": "Noun", "form": "Person", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a musician","a singer","an American singer"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
+      </c>
+      <c r="B800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",U800,""",""",V800,""",""",W800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="C800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",X800,""",""",Y800,""",""",Z800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="D800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AA800,""",""",AB800,""",""",AC800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="E800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AD800,""",""",AE800,""",""",AF800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="F800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AG800,""",""",AH800,""",""",AI800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="G800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AJ800,""",""",AK800,""",""",AL800,""""),",""""",""),"""""","")</f>
+        <v>"a musician","a singer","an American singer"</v>
+      </c>
+      <c r="H800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AM800,""",""",AN800,""",""",AO800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="I800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AP800,""",""",AQ800,""",""",AR800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="J800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AS800,""",""",AT800,""",""",AU800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="K800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AV800,""",""",AW800,""",""",AX800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="L800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AY800,""",""",AZ800,""",""",BA800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="M800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",BB800,""",""",BC800,""",""",BD800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="N800" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",BE800,""",""",BF800,""",""",BG800,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="O800" s="1"/>
+      <c r="Q800" s="1" t="s">
+        <v>1728</v>
+      </c>
+      <c r="S800" t="s">
+        <v>0</v>
+      </c>
+      <c r="T800" t="s">
+        <v>1727</v>
+      </c>
+      <c r="AJ800" t="s">
+        <v>1379</v>
+      </c>
+      <c r="AK800" t="s">
+        <v>1046</v>
+      </c>
+      <c r="AL800" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="801" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A801" t="str">
+        <f>CONCATENATE("{""spelling"": """,Q801,""", ""group"": """,O801,""", ""pos"": """,S801,""", ""form"": """,T801,""", ""adult"": ",IF(R801=TRUE,"true","false"),", ""has"": [",B801,"]",", ""in"": [",C801,"]",", ""on"": [",D801,"]",", ""from"": [",E801,"]",", ""is"": [",F801,"]",", ""typeOf"": [",G801,"]",", ""supertypeOf"": [",H801,"]",", ""nearlyIs"": [",I801,"]",", ""property"": [",J801,"]",", ""acts"": [",K801,"]",", ""actsCont"": [",L801,"]",", ""recipient"": [",M801,"]",", ""recipientPast"": [",N801,"]},")</f>
+        <v>{"spelling": "James Brown", "group": "", "pos": "Noun", "form": "Person", "adult": false, "has": [], "in": [], "on": [], "from": [], "is": [], "typeOf": ["a musician","a singer","an American singer"], "supertypeOf": [], "nearlyIs": [], "property": [], "acts": [], "actsCont": [], "recipient": [], "recipientPast": []},</v>
+      </c>
+      <c r="B801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",U801,""",""",V801,""",""",W801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="C801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",X801,""",""",Y801,""",""",Z801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="D801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AA801,""",""",AB801,""",""",AC801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="E801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AD801,""",""",AE801,""",""",AF801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="F801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AG801,""",""",AH801,""",""",AI801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="G801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AJ801,""",""",AK801,""",""",AL801,""""),",""""",""),"""""","")</f>
+        <v>"a musician","a singer","an American singer"</v>
+      </c>
+      <c r="H801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AM801,""",""",AN801,""",""",AO801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="I801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AP801,""",""",AQ801,""",""",AR801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="J801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AS801,""",""",AT801,""",""",AU801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="K801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AV801,""",""",AW801,""",""",AX801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="L801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",AY801,""",""",AZ801,""",""",BA801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="M801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",BB801,""",""",BC801,""",""",BD801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="N801" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("""",BE801,""",""",BF801,""",""",BG801,""""),",""""",""),"""""","")</f>
+        <v/>
+      </c>
+      <c r="O801" s="1"/>
+      <c r="Q801" s="1" t="s">
+        <v>1729</v>
+      </c>
+      <c r="S801" t="s">
+        <v>0</v>
+      </c>
+      <c r="T801" t="s">
+        <v>1727</v>
+      </c>
+      <c r="AJ801" t="s">
+        <v>1379</v>
+      </c>
+      <c r="AK801" t="s">
+        <v>1046</v>
+      </c>
+      <c r="AL801" t="s">
+        <v>1654</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>